<commit_message>
correct rotation of p&p'd parts.
</commit_message>
<xml_diff>
--- a/Hardware/stm32-pi_full/stm32 v1.0 working BoM/JLCSMT_Sample_BOM1.xlsx
+++ b/Hardware/stm32-pi_full/stm32 v1.0 working BoM/JLCSMT_Sample_BOM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d4/Documents/github/emonSTM32-db/Hardware/stm32-pi_full/stm32 v1.0 working BoM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702437D8-25B1-7E4A-A56F-140AA1BFE2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27915BB-CC50-6544-AA3F-1C07B9D14EF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="206">
   <si>
     <t>Comment</t>
   </si>
@@ -564,9 +564,6 @@
     <t>RF9</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>ESD5Z3.3T1G</t>
   </si>
   <si>
@@ -576,15 +573,6 @@
     <t>AP7313-33SRG-7</t>
   </si>
   <si>
-    <t>Green 1.85V</t>
-  </si>
-  <si>
-    <t>Orange 1.85V</t>
-  </si>
-  <si>
-    <t>Red 1.85V</t>
-  </si>
-  <si>
     <t>LMV824IDG4</t>
   </si>
   <si>
@@ -603,9 +591,6 @@
     <t>6R8</t>
   </si>
   <si>
-    <t>KSS221GLFS</t>
-  </si>
-  <si>
     <t>C0603</t>
   </si>
   <si>
@@ -624,9 +609,6 @@
     <t>SOT96P240X135-3N</t>
   </si>
   <si>
-    <t>CHIP-LED0805</t>
-  </si>
-  <si>
     <t>SOIC127P600X175-14N</t>
   </si>
   <si>
@@ -642,9 +624,6 @@
     <t>R0805</t>
   </si>
   <si>
-    <t>KSS</t>
-  </si>
-  <si>
     <t>ferrite</t>
   </si>
   <si>
@@ -652,6 +631,18 @@
   </si>
   <si>
     <t>npn</t>
+  </si>
+  <si>
+    <t>LED 0805</t>
+  </si>
+  <si>
+    <t>white led 0805 C34499</t>
+  </si>
+  <si>
+    <t>yellow led 0805 C2296</t>
+  </si>
+  <si>
+    <t>red led 0805 C84256</t>
   </si>
 </sst>
 </file>
@@ -670,7 +661,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1045,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1078,7 +1069,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" customHeight="1">
@@ -1089,7 +1080,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" customHeight="1">
@@ -1100,7 +1091,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1111,7 +1102,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1122,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1133,7 +1124,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1144,7 +1135,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1155,7 +1146,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1166,7 +1157,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1177,7 +1168,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1188,7 +1179,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1199,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1210,7 +1201,7 @@
         <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1221,7 +1212,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1232,7 +1223,7 @@
         <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1243,7 +1234,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1254,7 +1245,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1265,7 +1256,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1276,7 +1267,7 @@
         <v>55</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1287,7 +1278,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1298,7 +1289,7 @@
         <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1309,7 +1300,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1320,7 +1311,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1331,7 +1322,7 @@
         <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1342,7 +1333,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1353,7 +1344,7 @@
         <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1364,7 +1355,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1375,7 +1366,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1386,7 +1377,7 @@
         <v>65</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1397,7 +1388,7 @@
         <v>66</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1408,7 +1399,7 @@
         <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1419,7 +1410,7 @@
         <v>68</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1430,7 +1421,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1441,7 +1432,7 @@
         <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1452,7 +1443,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1463,7 +1454,7 @@
         <v>72</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1474,7 +1465,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1485,7 +1476,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1496,7 +1487,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1507,7 +1498,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1518,7 +1509,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1529,7 +1520,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1540,7 +1531,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1551,7 +1542,7 @@
         <v>79</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1562,7 +1553,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1573,7 +1564,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1584,7 +1575,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1595,7 +1586,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1606,7 +1597,7 @@
         <v>83</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1617,7 +1608,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1628,7 +1619,7 @@
         <v>85</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1639,7 +1630,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1650,7 +1641,7 @@
         <v>87</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1661,7 +1652,7 @@
         <v>88</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1672,7 +1663,7 @@
         <v>89</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1683,7 +1674,7 @@
         <v>90</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1694,7 +1685,7 @@
         <v>91</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1705,7 +1696,7 @@
         <v>92</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1716,271 +1707,271 @@
         <v>93</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1991,7 +1982,7 @@
         <v>118</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2002,7 +1993,7 @@
         <v>119</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2013,7 +2004,7 @@
         <v>30</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2024,7 +2015,7 @@
         <v>120</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2035,7 +2026,7 @@
         <v>121</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2046,7 +2037,7 @@
         <v>26</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2057,7 +2048,7 @@
         <v>34</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2068,7 +2059,7 @@
         <v>37</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2079,7 +2070,7 @@
         <v>24</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2090,7 +2081,7 @@
         <v>122</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2101,7 +2092,7 @@
         <v>123</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2112,7 +2103,7 @@
         <v>124</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2123,7 +2114,7 @@
         <v>125</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2134,7 +2125,7 @@
         <v>126</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2145,7 +2136,7 @@
         <v>127</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2156,7 +2147,7 @@
         <v>128</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2167,7 +2158,7 @@
         <v>129</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2178,7 +2169,7 @@
         <v>130</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2189,7 +2180,7 @@
         <v>131</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2200,7 +2191,7 @@
         <v>132</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2211,7 +2202,7 @@
         <v>133</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2222,7 +2213,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2233,7 +2224,7 @@
         <v>134</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2244,7 +2235,7 @@
         <v>21</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2255,7 +2246,7 @@
         <v>135</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2266,7 +2257,7 @@
         <v>136</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2277,29 +2268,29 @@
         <v>137</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2310,29 +2301,29 @@
         <v>140</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2343,7 +2334,7 @@
         <v>143</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2354,7 +2345,7 @@
         <v>144</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2365,7 +2356,7 @@
         <v>145</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2376,7 +2367,7 @@
         <v>146</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2387,7 +2378,7 @@
         <v>147</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2398,7 +2389,7 @@
         <v>148</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2409,7 +2400,7 @@
         <v>149</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2420,7 +2411,7 @@
         <v>150</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2431,7 +2422,7 @@
         <v>151</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2442,7 +2433,7 @@
         <v>152</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2453,7 +2444,7 @@
         <v>153</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2464,7 +2455,7 @@
         <v>154</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2475,18 +2466,18 @@
         <v>155</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2497,7 +2488,7 @@
         <v>157</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2508,7 +2499,7 @@
         <v>158</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2519,7 +2510,7 @@
         <v>159</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2530,7 +2521,7 @@
         <v>160</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2541,106 +2532,106 @@
         <v>32</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2651,7 +2642,7 @@
         <v>170</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2662,7 +2653,7 @@
         <v>171</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2673,7 +2664,7 @@
         <v>172</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2684,7 +2675,7 @@
         <v>173</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2695,7 +2686,7 @@
         <v>174</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2706,7 +2697,7 @@
         <v>175</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2717,7 +2708,7 @@
         <v>176</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2728,7 +2719,7 @@
         <v>177</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2739,18 +2730,7 @@
         <v>178</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>